<commit_message>
1) atualizar testes da marjan;
</commit_message>
<xml_diff>
--- a/CoParticipacaoWebService/src/test/resources/marjan/input/MARJAN.NAO-LOCALIZADO.201808.004.xlsx
+++ b/CoParticipacaoWebService/src/test/resources/marjan/input/MARJAN.NAO-LOCALIZADO.201808.004.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="50">
   <si>
     <t xml:space="preserve">ID TITULAR</t>
   </si>
@@ -43,10 +43,34 @@
     <t xml:space="preserve">DEMITIDOS</t>
   </si>
   <si>
-    <t xml:space="preserve">EDSON JOSE NUNES DA SILVA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MIGUEL NUNES DE SOUZA</t>
+    <t xml:space="preserve">EDICARLOS BARRETO SILVA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CARLOS HENRIQUE B SILVA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ODAIR JOSE DA SILVA LIMA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRISCILA GARCIA DE OLIVEIRA LIMA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SARA MARIA DA CRUZ R M ASSIS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADRIANO CALIXTO COSTA DOS SANTOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JUCILENE DA SILVA C C DOS SANTOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALINE VILELA DE SIQUEIRA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANTONIO VAGNER FARIAS GOMES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EDUARDA KEMILLY OLIVEIRA FARIAS</t>
   </si>
   <si>
     <t xml:space="preserve">CARLA CRISTINA V DEFAVARI</t>
@@ -55,12 +79,36 @@
     <t xml:space="preserve">BEATRIZ VENDRAMEL BORGES</t>
   </si>
   <si>
+    <t xml:space="preserve">KAMILA JESSICA PEREIRA NOGUEIRA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MARIA ALICE DIONISIO PEREIRA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MARIA CLARA DIONISIO PEREIRA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KELLY GOMES L GALVAO MONTEIRO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RODRIGO FELIX MONTEIRO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LILIAN PIERRI MARTINS</t>
+  </si>
+  <si>
     <t xml:space="preserve">LIVIA DE ANDRADE</t>
   </si>
   <si>
     <t xml:space="preserve">FELIPE AUGUSTO ANDRADE DE JESUS</t>
   </si>
   <si>
+    <t xml:space="preserve">LUIZ CARLOS MOREIRA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROSIMEIRE A DOS SANTOS MOREIRA</t>
+  </si>
+  <si>
     <t xml:space="preserve">MARIA APARECIDA DE ALBUQUERQUE</t>
   </si>
   <si>
@@ -73,73 +121,58 @@
     <t xml:space="preserve">GUILHERME FERREIRA BEZERRA</t>
   </si>
   <si>
-    <t xml:space="preserve">ISABELA DE LIMA SANTOS LYRA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HEITOR LYRA DOS SANTOS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SHEILA DA CRUZ NOVAES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LETICIA CRUZ DOS SANTOS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JANAINA SEVERINA DA SILVA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LETYCIA SILVA E SILVA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KAMILA JESSICA PEREIRA NOGUEIRA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MARIA ALICE DIONISIO PEREIRA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MARCOS ANDRE KAPOR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MARIA CLARA BIANCO KAPOR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MARIA CLARA DIONISIO PEREIRA</t>
-  </si>
-  <si>
     <t xml:space="preserve">MIRIAM VIEIRA PIRES SILVA</t>
   </si>
   <si>
     <t xml:space="preserve">MURILO PIRES SUPESCHI GONCALVES</t>
   </si>
   <si>
-    <t xml:space="preserve">ANDERSON ALEX APOLINARIO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RAFAELA CORREA APOLINARIO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KELLY GOMES L GALVAO MONTEIRO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RODRIGO FELIX MONTEIRO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LUIZ CARLOS MOREIRA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ROSIMEIRE A DOS SANTOS MOREIRA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WILLIAN DE MELO MATTOS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STEPHANY EDUARDO MATTOS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EDUARDO MORAES DOS SANTOS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TOMAZ CASTELLANI SANTOS</t>
+    <t xml:space="preserve">RICARDO DE BRITO ANDRADE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIDIANY MONIKE CALIXTO DE BRITO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROBSON RICETO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STEFANO ROBERTO DA SILVA B ELIAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SARITA RUGGIERI Z CAMPINEIRO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WELLINGTON ZACCARELLI CAMPINEIRO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEMAIAS MAISTRO LEITE CUSTODIO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NATALLIA SOARES SILVA CUSTODIO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TATIANA BATISTA DA SILVA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NICOLAS RODRIGUES BATISTA DA SIL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VANESSA DA FONSECA ROSAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VERA REGINA CERIOLI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CARLOS SANTOS DIAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VIVIANE DE LIMA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WAGNER LUCIO RESTINO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SILVIA HELENA DE FREITAS RESTINO</t>
   </si>
 </sst>
 </file>
@@ -150,11 +183,12 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -182,6 +216,19 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -239,7 +286,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -253,6 +300,22 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -333,13 +396,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="27.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="54.69"/>
@@ -348,7 +411,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.67"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -368,21 +431,39 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
-        <v>40</v>
+        <v>74</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>38257380865</v>
+        <v>27428718880</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="3" t="n">
-        <v>45001</v>
+        <v>450000</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="n">
+        <v>63</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>26586645832</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="3" t="n">
+        <f aca="false">D2+1</f>
+        <v>450001</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -401,39 +482,56 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="27.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="54.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="27.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="54.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="4" width="27.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="4" width="54.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="4" width="27.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="4" width="54.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="4" width="8.67"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="n">
+        <v>21676118896</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="7" t="n">
+        <v>5500001</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -452,13 +550,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="27.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="54.69"/>
@@ -467,7 +565,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.67"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -487,108 +585,108 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
-        <v>3205</v>
+        <v>4100</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>47761092800</v>
+        <v>34975562898</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="3" t="n">
-        <v>75001</v>
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>650000</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="n">
-        <v>3948</v>
+        <v>4782</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>28525882852</v>
+        <v>31163949892</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="D3" s="2" t="n">
         <f aca="false">D2+1</f>
-        <v>75002</v>
+        <v>650001</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="n">
-        <v>4250</v>
+        <v>4365</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>5281592165</v>
+        <v>36396453835</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="D4" s="2" t="n">
         <f aca="false">D3+1</f>
-        <v>75003</v>
+        <v>650002</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="n">
-        <v>4353</v>
+        <v>3205</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>51884618898</v>
+        <v>47761092800</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="D5" s="2" t="n">
         <f aca="false">D4+1</f>
-        <v>75004</v>
+        <v>650003</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="n">
-        <v>4063</v>
+        <v>4368</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>10763539759</v>
+        <v>2896161155</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="3" t="n">
+        <v>18</v>
+      </c>
+      <c r="D6" s="2" t="n">
         <f aca="false">D5+1</f>
-        <v>75005</v>
+        <v>650004</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="n">
-        <v>3903</v>
+        <v>4368</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>34377946803</v>
+        <v>8149047182</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="3" t="n">
+      <c r="D7" s="2" t="n">
         <f aca="false">D6+1</f>
-        <v>75006</v>
+        <v>650005</v>
       </c>
       <c r="E7" s="0" t="s">
         <v>19</v>
@@ -596,182 +694,326 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="n">
-        <v>4247</v>
-      </c>
-      <c r="B8" s="2" t="n">
-        <v>22596126877</v>
+        <v>4368</v>
+      </c>
+      <c r="B8" s="3" t="n">
+        <v>41461180007</v>
       </c>
       <c r="C8" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <f aca="false">D7+1</f>
+        <v>650006</v>
+      </c>
+      <c r="E8" s="0" t="s">
         <v>20</v>
-      </c>
-      <c r="D8" s="3" t="n">
-        <f aca="false">D7+1</f>
-        <v>75007</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="n">
-        <v>4368</v>
+        <v>4164</v>
       </c>
       <c r="B9" s="2" t="n">
-        <v>8149047182</v>
+        <v>86798812104</v>
       </c>
       <c r="C9" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <f aca="false">D8+1</f>
+        <v>650007</v>
+      </c>
+      <c r="E9" s="0" t="s">
         <v>22</v>
-      </c>
-      <c r="D9" s="3" t="n">
-        <f aca="false">D8+1</f>
-        <v>75008</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="n">
-        <v>3262</v>
+        <v>4847</v>
       </c>
       <c r="B10" s="2" t="n">
-        <v>27012636890</v>
+        <v>18195967884</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="D10" s="2" t="n">
         <f aca="false">D9+1</f>
-        <v>75009</v>
+        <v>650008</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="n">
-        <v>4368</v>
-      </c>
-      <c r="B11" s="3" t="n">
-        <v>4481934000</v>
+        <v>3948</v>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>28525882852</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="D11" s="2" t="n">
         <f aca="false">D10+1</f>
-        <v>75010</v>
+        <v>650009</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="n">
-        <v>4286</v>
+        <v>4037</v>
       </c>
       <c r="B12" s="2" t="n">
-        <v>19682736897</v>
+        <v>11644614863</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="D12" s="2" t="n">
         <f aca="false">D11+1</f>
-        <v>75011</v>
+        <v>650010</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="n">
-        <v>4532</v>
+        <v>4037</v>
       </c>
       <c r="B13" s="2" t="n">
-        <v>16667804809</v>
+        <v>5426606609</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="D13" s="2" t="n">
         <f aca="false">D12+1</f>
-        <v>75012</v>
+        <v>650011</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="n">
-        <v>4164</v>
+        <v>4250</v>
       </c>
       <c r="B14" s="2" t="n">
-        <v>86798812104</v>
+        <v>5281592165</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="D14" s="2" t="n">
         <f aca="false">D13+1</f>
-        <v>75013</v>
+        <v>650012</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="n">
-        <v>4037</v>
+        <v>4353</v>
       </c>
       <c r="B15" s="2" t="n">
-        <v>5426606609</v>
+        <v>51884618898</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="D15" s="2" t="n">
         <f aca="false">D14+1</f>
-        <v>75014</v>
+        <v>650013</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="n">
-        <v>4136</v>
+        <v>4286</v>
       </c>
       <c r="B16" s="2" t="n">
-        <v>8641947736</v>
+        <v>19682736897</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="3" t="n">
+        <v>32</v>
+      </c>
+      <c r="D16" s="2" t="n">
         <f aca="false">D15+1</f>
-        <v>75015</v>
+        <v>650014</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="n">
-        <v>3173</v>
+        <v>4900</v>
       </c>
       <c r="B17" s="2" t="n">
-        <v>15131400864</v>
+        <v>37060975837</v>
       </c>
       <c r="C17" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="2" t="n">
+        <f aca="false">D16+1</f>
+        <v>650015</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="n">
+        <v>4357</v>
+      </c>
+      <c r="B18" s="2" t="n">
+        <v>6118559848</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="2" t="n">
+        <f aca="false">D17+1</f>
+        <v>650016</v>
+      </c>
+      <c r="E18" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="3" t="n">
-        <f aca="false">D16+1</f>
-        <v>75016</v>
-      </c>
-      <c r="E17" s="0" t="s">
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2" t="n">
+        <v>3176</v>
+      </c>
+      <c r="B19" s="2" t="n">
+        <v>8440800800</v>
+      </c>
+      <c r="C19" s="0" t="s">
         <v>38</v>
+      </c>
+      <c r="D19" s="2" t="n">
+        <f aca="false">D18+1</f>
+        <v>650017</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="n">
+        <v>4905</v>
+      </c>
+      <c r="B20" s="2" t="n">
+        <v>35952321860</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="2" t="n">
+        <f aca="false">D19+1</f>
+        <v>650018</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="n">
+        <v>4509</v>
+      </c>
+      <c r="B21" s="2" t="n">
+        <v>35280916811</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="2" t="n">
+        <f aca="false">D20+1</f>
+        <v>650019</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2" t="n">
+        <v>4372</v>
+      </c>
+      <c r="B22" s="2" t="n">
+        <v>36835601850</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" s="2" t="n">
+        <f aca="false">D21+1</f>
+        <v>650020</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2" t="n">
+        <v>2249</v>
+      </c>
+      <c r="B23" s="2" t="n">
+        <v>23163690068</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" s="2" t="n">
+        <f aca="false">D22+1</f>
+        <v>650021</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="2" t="n">
+        <v>4904</v>
+      </c>
+      <c r="B24" s="2" t="n">
+        <v>30961892854</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="2" t="n">
+        <f aca="false">D23+1</f>
+        <v>650022</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="2" t="n">
+        <v>4622</v>
+      </c>
+      <c r="B25" s="2" t="n">
+        <v>6518293802</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="D25" s="2" t="n">
+        <f aca="false">D24+1</f>
+        <v>650023</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>